<commit_message>
Updates to fix formatting of exported SharePoint values. Customized scrollbars for uniformity of aesthetics.
</commit_message>
<xml_diff>
--- a/Publish/Resources/2048-980-3256.PFS_Surgical Skin Prep_Final-4.12.2021 (1).xlsx
+++ b/Publish/Resources/2048-980-3256.PFS_Surgical Skin Prep_Final-4.12.2021 (1).xlsx
@@ -3944,9 +3944,10 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100364BA8222640BF40B47B20B9F827EE1E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2cebb18baacb12859fd3da58e6915a65">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="51796436-8a0c-435a-829e-18e6ae7f62dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f2b2d5c17d217e7e550298babebd8ee" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100364BA8222640BF40B47B20B9F827EE1E" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70f4daa53e4b9068220a121fed56b974">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="51796436-8a0c-435a-829e-18e6ae7f62dc" xmlns:ns3="e6bdf5ed-f06e-4a49-88e7-9a55df091a23" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b295c49f26fcbb8c0bc28ceaa9e38025" ns2:_="" ns3:_="">
     <xsd:import namespace="51796436-8a0c-435a-829e-18e6ae7f62dc"/>
+    <xsd:import namespace="e6bdf5ed-f06e-4a49-88e7-9a55df091a23"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -3955,6 +3956,10 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3973,6 +3978,48 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e6bdf5ed-f06e-4a49-88e7-9a55df091a23" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4084,5 +4131,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EAB3357-CA58-40B7-A1EA-F536E2971018}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73CDC021-F42E-4480-AF96-EA6AEAF72438}"/>
 </file>
</xml_diff>

<commit_message>
Updated image link to Huddle
</commit_message>
<xml_diff>
--- a/Publish/Resources/2048-980-3256.PFS_Surgical Skin Prep_Final-4.12.2021 (1).xlsx
+++ b/Publish/Resources/2048-980-3256.PFS_Surgical Skin Prep_Final-4.12.2021 (1).xlsx
@@ -3930,7 +3930,10 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <Publish xmlns="51796436-8a0c-435a-829e-18e6ae7f62dc">false</Publish>
+    <Summary xmlns="51796436-8a0c-435a-829e-18e6ae7f62dc"/>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -3944,8 +3947,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100364BA8222640BF40B47B20B9F827EE1E" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70f4daa53e4b9068220a121fed56b974">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="51796436-8a0c-435a-829e-18e6ae7f62dc" xmlns:ns3="e6bdf5ed-f06e-4a49-88e7-9a55df091a23" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b295c49f26fcbb8c0bc28ceaa9e38025" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100364BA8222640BF40B47B20B9F827EE1E" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b87327e82458898bf34277b84cd0bd2b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="51796436-8a0c-435a-829e-18e6ae7f62dc" xmlns:ns3="e6bdf5ed-f06e-4a49-88e7-9a55df091a23" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="715944ce15a3d6808a1633d5a1e74cc9" ns2:_="" ns3:_="">
     <xsd:import namespace="51796436-8a0c-435a-829e-18e6ae7f62dc"/>
     <xsd:import namespace="e6bdf5ed-f06e-4a49-88e7-9a55df091a23"/>
     <xsd:element name="properties">
@@ -3960,6 +3963,8 @@
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:Summary"/>
+                <xsd:element ref="ns2:Publish" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3990,6 +3995,18 @@
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Summary" ma:index="14" ma:displayName="Summary" ma:description="Summary of the contents in the document" ma:format="Dropdown" ma:internalName="Summary">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Publish" ma:index="15" nillable="true" ma:displayName="Publish" ma:default="0" ma:description="Visible to public" ma:format="Dropdown" ma:internalName="Publish">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4131,5 +4148,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73CDC021-F42E-4480-AF96-EA6AEAF72438}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF435B04-966C-4D19-82E7-ABA905E8DF72}"/>
 </file>
</xml_diff>